<commit_message>
Inspections transcriptions minor update
</commit_message>
<xml_diff>
--- a/BritishAssociationReports/BAAS_Inspections.xlsx
+++ b/BritishAssociationReports/BAAS_Inspections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\BritishAssociationReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AFF514-6963-4B93-B96C-B0BD33AE6B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1DEC1E-8698-4FBC-AD0D-1C0E1B5E29FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{165AC260-63B9-4BEA-BDF9-867FB820D959}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8048" uniqueCount="2939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8050" uniqueCount="2940">
   <si>
     <t>Report year</t>
   </si>
@@ -8869,6 +8869,9 @@
   </si>
   <si>
     <t>Leftover: EXETER-ALBERT-TERRACE-VICARY</t>
+  </si>
+  <si>
+    <t>Actually Kent not Sussex</t>
   </si>
 </sst>
 </file>
@@ -27020,10 +27023,10 @@
   <dimension ref="A1:S656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="O126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S147" sqref="S147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34510,7 +34513,7 @@
         <v>2925</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -34560,7 +34563,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -34613,7 +34616,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -34666,7 +34669,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -34719,7 +34722,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -34772,7 +34775,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -34822,7 +34825,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -34872,7 +34875,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -34925,7 +34928,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -34972,7 +34975,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -35021,8 +35024,11 @@
       <c r="R154" s="9" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S154" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -35068,8 +35074,11 @@
       <c r="R155" s="9" t="s">
         <v>1359</v>
       </c>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S155" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -35119,7 +35128,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -35172,7 +35181,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -35216,7 +35225,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -35272,7 +35281,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>

</xml_diff>